<commit_message>
excel data structure schema
</commit_message>
<xml_diff>
--- a/Book1-v2.xlsx
+++ b/Book1-v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mo\OneDrive\Data Analysis Faouzi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Classroom\Desktop\paython_adel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="65">
   <si>
     <t>'title'</t>
   </si>
@@ -218,6 +218,27 @@
   </si>
   <si>
     <t>count the Max occurrences and minimam occurrences</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>namespace}d</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -228,35 +249,35 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -264,21 +285,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -286,7 +307,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -294,21 +315,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -387,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -530,6 +551,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -540,7 +579,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
@@ -584,6 +623,102 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -593,111 +728,25 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Accent2" xfId="5" builtinId="33"/>
-    <cellStyle name="Accent5" xfId="6" builtinId="45"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="4" builtinId="10"/>
+    <cellStyle name="إدخال" xfId="3" builtinId="20"/>
+    <cellStyle name="تمييز2" xfId="5" builtinId="33"/>
+    <cellStyle name="تمييز5" xfId="6" builtinId="45"/>
+    <cellStyle name="جيد" xfId="1" builtinId="26"/>
+    <cellStyle name="سيئ" xfId="2" builtinId="27"/>
+    <cellStyle name="ملاحظة" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -717,7 +766,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="نسق Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -985,24 +1034,24 @@
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.25" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.125" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="3.42578125" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.375" customWidth="1"/>
+    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1016,7 +1065,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -1042,7 +1091,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1077,7 +1126,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1112,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1147,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +1234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1214,7 +1263,7 @@
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1294,7 @@
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -1318,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
@@ -1349,7 +1398,7 @@
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
@@ -1377,7 +1426,7 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1408,7 +1457,7 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>0</v>
       </c>
@@ -1443,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>11</v>
       </c>
@@ -1478,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>0</v>
       </c>
@@ -1507,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>4</v>
       </c>
@@ -1533,7 +1582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>2</v>
       </c>
@@ -1559,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>13</v>
       </c>
@@ -1573,7 +1622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>2</v>
       </c>
@@ -1587,7 +1636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>2</v>
       </c>
@@ -1601,7 +1650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>2</v>
       </c>
@@ -1626,114 +1675,128 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:Q23"/>
+  <dimension ref="C4:Q51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0.75" customWidth="1"/>
+    <col min="2" max="2" width="1.375" customWidth="1"/>
+    <col min="8" max="8" width="6.875" customWidth="1"/>
+    <col min="9" max="9" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.375" customWidth="1"/>
+    <col min="11" max="11" width="7.25" customWidth="1"/>
+    <col min="12" max="12" width="6" customWidth="1"/>
+    <col min="13" max="13" width="6.375" customWidth="1"/>
+    <col min="14" max="14" width="5.75" customWidth="1"/>
+    <col min="15" max="15" width="4.5" customWidth="1"/>
+    <col min="16" max="16" width="4.625" customWidth="1"/>
+    <col min="17" max="17" width="5.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>56</v>
       </c>
-      <c r="L4" t="s">
+      <c r="I4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C6" s="56" t="s">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C6" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="I6" s="58" t="s">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="I6" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-    </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-    </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C8" s="25" t="s">
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C8" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="57" t="s">
         <v>49</v>
       </c>
       <c r="H8" s="19"/>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="52" t="s">
+      <c r="J8" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="53"/>
-      <c r="L8" s="52" t="s">
+      <c r="K8" s="48"/>
+      <c r="L8" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="53"/>
-      <c r="N8" s="52" t="s">
+      <c r="M8" s="48"/>
+      <c r="N8" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="O8" s="53"/>
-      <c r="P8" s="52" t="s">
+      <c r="O8" s="48"/>
+      <c r="P8" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="Q8" s="53"/>
-    </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="Q8" s="48"/>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C9" s="58"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
       <c r="H9" s="19"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="55"/>
-    </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C10" s="27"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="50"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="50"/>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C10" s="59"/>
       <c r="D10" s="24">
         <v>3</v>
       </c>
@@ -1747,7 +1810,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="19"/>
-      <c r="I10" s="38"/>
+      <c r="I10" s="33"/>
       <c r="J10" s="20" t="s">
         <v>54</v>
       </c>
@@ -1773,24 +1836,24 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="28" t="s">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C11" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="29" t="s">
         <v>49</v>
       </c>
       <c r="H11" s="19"/>
-      <c r="I11" s="39"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
@@ -1800,35 +1863,35 @@
       <c r="P11" s="20"/>
       <c r="Q11" s="20"/>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="J12" s="48" t="s">
+      <c r="J12" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="49"/>
-      <c r="L12" s="48" t="s">
+      <c r="K12" s="44"/>
+      <c r="L12" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="M12" s="49"/>
-      <c r="N12" s="48" t="s">
+      <c r="M12" s="44"/>
+      <c r="N12" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="O12" s="49"/>
-      <c r="P12" s="48" t="s">
+      <c r="O12" s="44"/>
+      <c r="P12" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="Q12" s="49"/>
-    </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C13" s="30"/>
+      <c r="Q12" s="44"/>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C13" s="31"/>
       <c r="D13" s="23">
         <v>0</v>
       </c>
@@ -1842,34 +1905,34 @@
         <v>1</v>
       </c>
       <c r="H13" s="19"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="51"/>
-    </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C14" s="31" t="s">
+      <c r="I13" s="30"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="46"/>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C14" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="54" t="s">
         <v>49</v>
       </c>
       <c r="H14" s="19"/>
-      <c r="I14" s="29"/>
+      <c r="I14" s="30"/>
       <c r="J14" s="23" t="s">
         <v>54</v>
       </c>
@@ -1895,14 +1958,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C15" s="55"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="19"/>
-      <c r="I15" s="30"/>
+      <c r="I15" s="31"/>
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
@@ -1912,8 +1975,8 @@
       <c r="P15" s="23"/>
       <c r="Q15" s="23"/>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C16" s="33"/>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C16" s="56"/>
       <c r="D16" s="22">
         <v>3</v>
       </c>
@@ -1927,61 +1990,61 @@
         <v>3</v>
       </c>
       <c r="H16" s="19"/>
-      <c r="I16" s="31" t="s">
+      <c r="I16" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="44" t="s">
+      <c r="J16" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="K16" s="45"/>
-      <c r="L16" s="44" t="s">
+      <c r="K16" s="40"/>
+      <c r="L16" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="M16" s="45"/>
-      <c r="N16" s="44" t="s">
+      <c r="M16" s="40"/>
+      <c r="N16" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="45"/>
-      <c r="P16" s="44" t="s">
+      <c r="O16" s="40"/>
+      <c r="P16" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="Q16" s="45"/>
-    </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C17" s="34" t="s">
+      <c r="Q16" s="40"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C17" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="34" t="s">
+      <c r="G17" s="51" t="s">
         <v>49</v>
       </c>
       <c r="H17" s="19"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="47"/>
-    </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="42"/>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C18" s="53"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
       <c r="H18" s="19"/>
-      <c r="I18" s="32"/>
+      <c r="I18" s="55"/>
       <c r="J18" s="22" t="s">
         <v>54</v>
       </c>
@@ -2007,8 +2070,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C19" s="36"/>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C19" s="52"/>
       <c r="D19" s="21">
         <v>6</v>
       </c>
@@ -2022,7 +2085,7 @@
         <v>5</v>
       </c>
       <c r="H19" s="19"/>
-      <c r="I19" s="33"/>
+      <c r="I19" s="56"/>
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
@@ -2032,58 +2095,58 @@
       <c r="P19" s="22"/>
       <c r="Q19" s="22"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="40" t="s">
+      <c r="J20" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="K20" s="41"/>
-      <c r="L20" s="40" t="s">
+      <c r="K20" s="36"/>
+      <c r="L20" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="M20" s="41"/>
-      <c r="N20" s="40" t="s">
+      <c r="M20" s="36"/>
+      <c r="N20" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="O20" s="41"/>
-      <c r="P20" s="40" t="s">
+      <c r="O20" s="36"/>
+      <c r="P20" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="Q20" s="41"/>
-    </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q20" s="36"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="43"/>
-    </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I21" s="53"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="38"/>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
-      <c r="I22" s="35"/>
+      <c r="I22" s="53"/>
       <c r="J22" s="21" t="s">
         <v>54</v>
       </c>
@@ -2109,14 +2172,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
-      <c r="I23" s="36"/>
+      <c r="I23" s="52"/>
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
@@ -2126,8 +2189,327 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="21"/>
     </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>63</v>
+      </c>
+      <c r="M27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C28" s="67"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="61"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C29" s="68"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="66">
+        <v>1</v>
+      </c>
+      <c r="H29" s="66">
+        <v>1</v>
+      </c>
+      <c r="I29" s="63"/>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C30" s="69"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="65"/>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C31" s="67"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="61"/>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C32" s="68"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="66">
+        <v>5</v>
+      </c>
+      <c r="H32" s="66">
+        <v>5</v>
+      </c>
+      <c r="I32" s="63"/>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C33" s="69"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="65"/>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C34" s="67"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="61"/>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C35" s="68"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="66">
+        <v>1</v>
+      </c>
+      <c r="H35" s="66">
+        <v>1</v>
+      </c>
+      <c r="I35" s="63"/>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C36" s="69"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="65"/>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C37" s="67"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="61"/>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C38" s="68"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="66">
+        <v>1</v>
+      </c>
+      <c r="H38" s="66">
+        <v>1</v>
+      </c>
+      <c r="I38" s="63"/>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C39" s="69"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="65"/>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C40" s="67"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="60"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="61"/>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C41" s="68"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="G41" s="66">
+        <v>0</v>
+      </c>
+      <c r="H41" s="66">
+        <v>3</v>
+      </c>
+      <c r="I41" s="63"/>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C42" s="69"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
+      <c r="H42" s="64"/>
+      <c r="I42" s="65"/>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C43" s="67"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="61"/>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C44" s="68"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="66">
+        <v>0</v>
+      </c>
+      <c r="H44" s="66">
+        <v>1</v>
+      </c>
+      <c r="I44" s="63"/>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C45" s="69"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="65"/>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C46" s="67"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="61"/>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C47" s="68"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="66">
+        <v>1</v>
+      </c>
+      <c r="H47" s="66">
+        <v>1</v>
+      </c>
+      <c r="I47" s="63"/>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C48" s="69"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="64"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="65"/>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C49" s="67"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="61"/>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C50" s="68"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="G50" s="66">
+        <v>1</v>
+      </c>
+      <c r="H50" s="66">
+        <v>1</v>
+      </c>
+      <c r="I50" s="63"/>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C51" s="69"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="64"/>
+      <c r="H51" s="64"/>
+      <c r="I51" s="65"/>
+    </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="P8:Q9"/>
+    <mergeCell ref="N8:O9"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="L8:M9"/>
+    <mergeCell ref="J8:K9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
     <mergeCell ref="C6:G7"/>
     <mergeCell ref="I6:Q7"/>
     <mergeCell ref="I12:I15"/>
@@ -2144,34 +2526,8 @@
     <mergeCell ref="N12:O13"/>
     <mergeCell ref="L12:M13"/>
     <mergeCell ref="J12:K13"/>
-    <mergeCell ref="P8:Q9"/>
-    <mergeCell ref="N8:O9"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="J8:K9"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ver 4. step1 2 3 4 integrated
1st version of generation of ontology
</commit_message>
<xml_diff>
--- a/Book1-v2.xlsx
+++ b/Book1-v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Classroom\Desktop\paython_adel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mo\OneDrive\Data Analysis Faouzi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="58">
   <si>
     <t>'title'</t>
   </si>
@@ -218,27 +218,6 @@
   </si>
   <si>
     <t>count the Max occurrences and minimam occurrences</t>
-  </si>
-  <si>
-    <t>dataset</t>
-  </si>
-  <si>
-    <t>namespace}d</t>
-  </si>
-  <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
 </sst>
 </file>
@@ -249,35 +228,35 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -285,21 +264,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -307,7 +286,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -315,21 +294,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -408,7 +387,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -551,24 +530,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -579,7 +540,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
@@ -623,6 +584,99 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -635,118 +689,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
+    <cellStyle name="Accent2" xfId="5" builtinId="33"/>
+    <cellStyle name="Accent5" xfId="6" builtinId="45"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="إدخال" xfId="3" builtinId="20"/>
-    <cellStyle name="تمييز2" xfId="5" builtinId="33"/>
-    <cellStyle name="تمييز5" xfId="6" builtinId="45"/>
-    <cellStyle name="جيد" xfId="1" builtinId="26"/>
-    <cellStyle name="سيئ" xfId="2" builtinId="27"/>
-    <cellStyle name="ملاحظة" xfId="4" builtinId="10"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -766,7 +717,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="نسق Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1034,24 +985,24 @@
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.25" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="8" max="8" width="9.125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="3.375" customWidth="1"/>
-    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.42578125" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1065,7 +1016,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -1091,7 +1042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1077,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1196,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -1234,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1263,7 +1214,7 @@
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1245,7 @@
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -1332,7 +1283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -1367,7 +1318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
@@ -1398,7 +1349,7 @@
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
     </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
@@ -1426,7 +1377,7 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1457,7 +1408,7 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>11</v>
       </c>
@@ -1527,7 +1478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>4</v>
       </c>
@@ -1582,7 +1533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>2</v>
       </c>
@@ -1608,7 +1559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>13</v>
       </c>
@@ -1622,7 +1573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>2</v>
       </c>
@@ -1636,7 +1587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>2</v>
       </c>
@@ -1650,7 +1601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>2</v>
       </c>
@@ -1675,128 +1626,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:Q51"/>
+  <dimension ref="C4:Q23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="0.75" customWidth="1"/>
-    <col min="2" max="2" width="1.375" customWidth="1"/>
-    <col min="8" max="8" width="6.875" customWidth="1"/>
-    <col min="9" max="9" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.375" customWidth="1"/>
-    <col min="11" max="11" width="7.25" customWidth="1"/>
-    <col min="12" max="12" width="6" customWidth="1"/>
-    <col min="13" max="13" width="6.375" customWidth="1"/>
-    <col min="14" max="14" width="5.75" customWidth="1"/>
-    <col min="15" max="15" width="4.5" customWidth="1"/>
-    <col min="16" max="16" width="4.625" customWidth="1"/>
-    <col min="17" max="17" width="5.75" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>56</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C6" s="25" t="s">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C6" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="I6" s="27" t="s">
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="I6" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-    </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-    </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C8" s="57" t="s">
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C8" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="25" t="s">
         <v>49</v>
       </c>
       <c r="H8" s="19"/>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="48"/>
-      <c r="L8" s="47" t="s">
+      <c r="K8" s="53"/>
+      <c r="L8" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="48"/>
-      <c r="N8" s="47" t="s">
+      <c r="M8" s="53"/>
+      <c r="N8" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="O8" s="48"/>
-      <c r="P8" s="47" t="s">
+      <c r="O8" s="53"/>
+      <c r="P8" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="Q8" s="48"/>
-    </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C9" s="58"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
+      <c r="Q8" s="53"/>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="19"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="50"/>
-    </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C10" s="59"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="55"/>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="27"/>
       <c r="D10" s="24">
         <v>3</v>
       </c>
@@ -1810,7 +1747,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="19"/>
-      <c r="I10" s="33"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="20" t="s">
         <v>54</v>
       </c>
@@ -1836,24 +1773,24 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C11" s="29" t="s">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C11" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="28" t="s">
         <v>49</v>
       </c>
       <c r="H11" s="19"/>
-      <c r="I11" s="34"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
@@ -1863,35 +1800,35 @@
       <c r="P11" s="20"/>
       <c r="Q11" s="20"/>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="29" t="s">
+      <c r="I12" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="J12" s="43" t="s">
+      <c r="J12" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="44"/>
-      <c r="L12" s="43" t="s">
+      <c r="K12" s="49"/>
+      <c r="L12" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="M12" s="44"/>
-      <c r="N12" s="43" t="s">
+      <c r="M12" s="49"/>
+      <c r="N12" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="O12" s="44"/>
-      <c r="P12" s="43" t="s">
+      <c r="O12" s="49"/>
+      <c r="P12" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="Q12" s="44"/>
-    </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C13" s="31"/>
+      <c r="Q12" s="49"/>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="30"/>
       <c r="D13" s="23">
         <v>0</v>
       </c>
@@ -1905,34 +1842,34 @@
         <v>1</v>
       </c>
       <c r="H13" s="19"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="46"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="46"/>
-    </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C14" s="54" t="s">
+      <c r="I13" s="29"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="51"/>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C14" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="54" t="s">
+      <c r="G14" s="31" t="s">
         <v>49</v>
       </c>
       <c r="H14" s="19"/>
-      <c r="I14" s="30"/>
+      <c r="I14" s="29"/>
       <c r="J14" s="23" t="s">
         <v>54</v>
       </c>
@@ -1958,14 +1895,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C15" s="55"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="19"/>
-      <c r="I15" s="31"/>
+      <c r="I15" s="30"/>
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
@@ -1975,8 +1912,8 @@
       <c r="P15" s="23"/>
       <c r="Q15" s="23"/>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C16" s="56"/>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="33"/>
       <c r="D16" s="22">
         <v>3</v>
       </c>
@@ -1990,61 +1927,61 @@
         <v>3</v>
       </c>
       <c r="H16" s="19"/>
-      <c r="I16" s="54" t="s">
+      <c r="I16" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="J16" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="K16" s="40"/>
-      <c r="L16" s="39" t="s">
+      <c r="K16" s="45"/>
+      <c r="L16" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="M16" s="40"/>
-      <c r="N16" s="39" t="s">
+      <c r="M16" s="45"/>
+      <c r="N16" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="40"/>
-      <c r="P16" s="39" t="s">
+      <c r="O16" s="45"/>
+      <c r="P16" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="Q16" s="40"/>
-    </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C17" s="51" t="s">
+      <c r="Q16" s="45"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C17" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="51" t="s">
+      <c r="G17" s="34" t="s">
         <v>49</v>
       </c>
       <c r="H17" s="19"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="42"/>
-    </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C18" s="53"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="47"/>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
       <c r="H18" s="19"/>
-      <c r="I18" s="55"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="22" t="s">
         <v>54</v>
       </c>
@@ -2070,8 +2007,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C19" s="52"/>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C19" s="36"/>
       <c r="D19" s="21">
         <v>6</v>
       </c>
@@ -2085,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="H19" s="19"/>
-      <c r="I19" s="56"/>
+      <c r="I19" s="33"/>
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
@@ -2095,58 +2032,58 @@
       <c r="P19" s="22"/>
       <c r="Q19" s="22"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
-      <c r="I20" s="51" t="s">
+      <c r="I20" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="35" t="s">
+      <c r="J20" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="K20" s="36"/>
-      <c r="L20" s="35" t="s">
+      <c r="K20" s="41"/>
+      <c r="L20" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="M20" s="36"/>
-      <c r="N20" s="35" t="s">
+      <c r="M20" s="41"/>
+      <c r="N20" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="O20" s="36"/>
-      <c r="P20" s="35" t="s">
+      <c r="O20" s="41"/>
+      <c r="P20" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="Q20" s="36"/>
-    </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="Q20" s="41"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="38"/>
-    </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="I21" s="35"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="43"/>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
-      <c r="I22" s="53"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="21" t="s">
         <v>54</v>
       </c>
@@ -2172,14 +2109,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
-      <c r="I23" s="52"/>
+      <c r="I23" s="36"/>
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
@@ -2189,327 +2126,8 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="21"/>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="E26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="L27" t="s">
-        <v>63</v>
-      </c>
-      <c r="M27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C28" s="67"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="61"/>
-    </row>
-    <row r="29" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C29" s="68"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="G29" s="66">
-        <v>1</v>
-      </c>
-      <c r="H29" s="66">
-        <v>1</v>
-      </c>
-      <c r="I29" s="63"/>
-    </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C30" s="69"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="65"/>
-    </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C31" s="67"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="61"/>
-    </row>
-    <row r="32" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C32" s="68"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="66">
-        <v>5</v>
-      </c>
-      <c r="H32" s="66">
-        <v>5</v>
-      </c>
-      <c r="I32" s="63"/>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C33" s="69"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="65"/>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C34" s="67"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="60"/>
-      <c r="I34" s="61"/>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C35" s="68"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="F35" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="G35" s="66">
-        <v>1</v>
-      </c>
-      <c r="H35" s="66">
-        <v>1</v>
-      </c>
-      <c r="I35" s="63"/>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C36" s="69"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="65"/>
-    </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C37" s="67"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="61"/>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C38" s="68"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="F38" s="66" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38" s="66">
-        <v>1</v>
-      </c>
-      <c r="H38" s="66">
-        <v>1</v>
-      </c>
-      <c r="I38" s="63"/>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C39" s="69"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="65"/>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C40" s="67"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="61"/>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C41" s="68"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="F41" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="G41" s="66">
-        <v>0</v>
-      </c>
-      <c r="H41" s="66">
-        <v>3</v>
-      </c>
-      <c r="I41" s="63"/>
-    </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C42" s="69"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="64"/>
-      <c r="F42" s="64"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="64"/>
-      <c r="I42" s="65"/>
-    </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C43" s="67"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="60"/>
-      <c r="H43" s="60"/>
-      <c r="I43" s="61"/>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C44" s="68"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="F44" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="G44" s="66">
-        <v>0</v>
-      </c>
-      <c r="H44" s="66">
-        <v>1</v>
-      </c>
-      <c r="I44" s="63"/>
-    </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C45" s="69"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="65"/>
-    </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C46" s="67"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="60"/>
-      <c r="H46" s="60"/>
-      <c r="I46" s="61"/>
-    </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C47" s="68"/>
-      <c r="D47" s="62"/>
-      <c r="E47" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="F47" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="G47" s="66">
-        <v>1</v>
-      </c>
-      <c r="H47" s="66">
-        <v>1</v>
-      </c>
-      <c r="I47" s="63"/>
-    </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C48" s="69"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="64"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="65"/>
-    </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C49" s="67"/>
-      <c r="D49" s="60"/>
-      <c r="E49" s="60"/>
-      <c r="F49" s="60"/>
-      <c r="G49" s="60"/>
-      <c r="H49" s="60"/>
-      <c r="I49" s="61"/>
-    </row>
-    <row r="50" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C50" s="68"/>
-      <c r="D50" s="62"/>
-      <c r="E50" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="F50" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="G50" s="66">
-        <v>1</v>
-      </c>
-      <c r="H50" s="66">
-        <v>1</v>
-      </c>
-      <c r="I50" s="63"/>
-    </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C51" s="69"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="65"/>
-    </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="P8:Q9"/>
-    <mergeCell ref="N8:O9"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="J8:K9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
     <mergeCell ref="C6:G7"/>
     <mergeCell ref="I6:Q7"/>
     <mergeCell ref="I12:I15"/>
@@ -2526,8 +2144,34 @@
     <mergeCell ref="N12:O13"/>
     <mergeCell ref="L12:M13"/>
     <mergeCell ref="J12:K13"/>
+    <mergeCell ref="P8:Q9"/>
+    <mergeCell ref="N8:O9"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="L8:M9"/>
+    <mergeCell ref="J8:K9"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>